<commit_message>
chore: updation of bca tt 62
</commit_message>
<xml_diff>
--- a/raw/time_tables/BCA(bca-62)/3/1.xlsx
+++ b/raw/time_tables/BCA(bca-62)/3/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="144">
   <si>
     <t>Bachelors of Computer Applications</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>LBCA1, BCA2(23B61CA211)-325/KSA</t>
+  </si>
+  <si>
     <t>LBCA3, BCA4(23B61CA213)-CR501/DCH</t>
   </si>
   <si>
@@ -64,27 +67,27 @@
     <t>PBCA4(23B65CA215)-CC423/IMR,REK</t>
   </si>
   <si>
+    <t>LBCA3, BCA4(23B61CA211)-CR526/KSA</t>
+  </si>
+  <si>
     <t>TBCA2(23B61CA212)-TR424/MEE</t>
   </si>
   <si>
     <t xml:space="preserve">
-PBCA2(23B65CA214)-CL317/RCN</t>
+PBCA2(23B65CA214)-CL317/SHG</t>
   </si>
   <si>
     <t>TBCA1(23B61CA212)-TR424/MEE</t>
   </si>
   <si>
     <t xml:space="preserve">
-PBCA1(23B65CA215)-CC417/AW,SON</t>
+PBCA1(23B65CA215)-CC417/AW</t>
   </si>
   <si>
     <t>TUE</t>
   </si>
   <si>
     <t>TBCA4(23B61CA212)-TR424/MEE</t>
-  </si>
-  <si>
-    <t>LBCA1, BCA2(23B61CA211)-CR301/ AKB</t>
   </si>
   <si>
     <t>LBCA3, BCA4(23B61CA212)-CR301/SHO</t>
@@ -99,13 +102,13 @@
     <t>PBCA2(23B65CA216)-CL24/AKT</t>
   </si>
   <si>
-    <t>PBCA3(23B65CA214)-CC423/SHP</t>
+    <t>PBCA3(23B65CA214)-CC423/KSA</t>
   </si>
   <si>
     <t>LBCA1, BCA2(23B61CA213)-CR325/DCH</t>
   </si>
   <si>
-    <t>PBCA4(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/SDA</t>
+    <t>PBCA4(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/BB</t>
   </si>
   <si>
     <t>WED</t>
@@ -114,10 +117,7 @@
     <t>LBCA1, BCA2(23B61CA212)-CR301/MEE</t>
   </si>
   <si>
-    <t>LBCA1, BCA2(23B61CA211)-325/AKB</t>
-  </si>
-  <si>
-    <t>LBCA1, BCA2(23B31HS211)-CR301/MSU</t>
+    <t>LBCA1, BCA2(23B31HS211)-CR301/SHU</t>
   </si>
   <si>
     <t>LBCA3, BCA4(23B61CS217)-CR301/ RJM</t>
@@ -126,13 +126,16 @@
     <t>LBCA3,BCA4(23B61CA212)-CR501/SHO</t>
   </si>
   <si>
-    <t>LBCA3, BCA4(23B61CA211)-CR325 AKB</t>
+    <t>LBCA3, BCA4(23B61CA211)-CR325 KSA</t>
   </si>
   <si>
-    <t>PBCA3(23B65CA215)-CC423/MEE,SON</t>
+    <t>PBCA3(23B65CA215)-CC423/MEE</t>
   </si>
   <si>
     <t>PBCA2(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/SDA</t>
+  </si>
+  <si>
+    <t>LBCA1, BCA2(23B61CA211)-CR301/ KSA</t>
   </si>
   <si>
     <t>THUR</t>
@@ -141,7 +144,7 @@
     <t>LBCA1, BCA2(23B31MA211)-CR301/HPT</t>
   </si>
   <si>
-    <t>LBCA1, BCA2(23B61CA211)-CR301/AKB</t>
+    <t>LBCA1, BCA2(23B61CA211)-CR301/KSA</t>
   </si>
   <si>
     <t>LBCA3, BCA4(23B61CS217)-CR501/RJM</t>
@@ -150,11 +153,11 @@
     <t>LBCA3, BCA4(23B31HS211)-CR301/SDA</t>
   </si>
   <si>
-    <t>PBCA4(23B65CA214)-CC417/AKB,DEE</t>
+    <t>PBCA4(23B65CA214)-CC417/KSA,DEE</t>
   </si>
   <si>
     <t xml:space="preserve">
-PBCA3( 23B65CA216)-CC417/DCH,AKT</t>
+PBCA3( 23B65CA216)-CL23/AKT</t>
   </si>
   <si>
     <t>LBCA1, BCA2(23B61CA212)-CR501/MEE</t>
@@ -163,7 +166,7 @@
     <t>TBCA3(23B61CA212)-TR326/MEE</t>
   </si>
   <si>
-    <t>PBCA4(23B65CA216)-CC423/PRK</t>
+    <t>PBCA4(23B65CA216)-CL24/PRK</t>
   </si>
   <si>
     <t>FRI</t>
@@ -178,7 +181,7 @@
     <t>LBCA3,BCA4(23B61CA212)-CR301/SHO</t>
   </si>
   <si>
-    <t>LBCA3, BCA4(23B61CA211)-CR 325/AKB</t>
+    <t>LBCA3, BCA4(23B61CA211)-CR 325/KSA</t>
   </si>
   <si>
     <t>LBCA3, BCA4(23B61CS217)-CR501/ RJM</t>
@@ -188,7 +191,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-PBCA1(23B65CA214)-CC421/AKB,RCN</t>
+PBCA1(23B65CA214)-CC421/SHG</t>
   </si>
   <si>
     <t>PBCA2(23B65CA215)-CC417/MEE,AW</t>
@@ -197,13 +200,10 @@
     <t>SAT</t>
   </si>
   <si>
-    <t>PBCA1(23B65CA216)-CC417/DCH</t>
+    <t>PBCA1(23B65CA216)-CL24/DCH</t>
   </si>
   <si>
-    <t>PBCA3(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/MSU</t>
-  </si>
-  <si>
-    <t>LBCA3, BCA4(23B61CA211)-CR526/AKB</t>
+    <t>PBCA3(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/SHU</t>
   </si>
   <si>
     <t xml:space="preserve">Faculty Abbreviation </t>
@@ -224,16 +224,28 @@
     <t>Prof Sandeep Kumar Singh</t>
   </si>
   <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>Dr. Suraj Das</t>
+  </si>
+  <si>
     <t>23B61CA211</t>
   </si>
   <si>
     <t>Algorithm and Problem Solving (APS)</t>
   </si>
   <si>
-    <t>AKB</t>
+    <t>KSA</t>
   </si>
   <si>
     <t>Aakriti Bhardwaj</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Dr. Badri Bajaj</t>
   </si>
   <si>
     <t>23B31MA211</t>
@@ -246,6 +258,12 @@
   </si>
   <si>
     <t>Shagun Gupta</t>
+  </si>
+  <si>
+    <t>SHU</t>
+  </si>
+  <si>
+    <t>Dr. Shubhayan</t>
   </si>
   <si>
     <t>23B61CA212</t>
@@ -878,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -905,7 +923,6 @@
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -924,6 +941,7 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="7" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -978,6 +996,12 @@
     <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf borderId="29" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -1008,9 +1032,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="29" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf borderId="9" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1407,22 +1428,24 @@
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1441,22 +1464,24 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="16"/>
+      <c r="G5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1475,20 +1500,20 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="13" t="s">
-        <v>19</v>
+      <c r="D6" s="12" t="s">
+        <v>21</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="18" t="s">
-        <v>20</v>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="17" t="s">
+        <v>22</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1516,7 +1541,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1536,31 +1561,29 @@
     </row>
     <row r="8">
       <c r="A8" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="E8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="G8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="16"/>
+      <c r="H8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -1580,23 +1603,23 @@
     </row>
     <row r="9">
       <c r="A9" s="24"/>
-      <c r="B9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="25" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="13" t="s">
-        <v>12</v>
+      <c r="E9" s="19"/>
+      <c r="F9" s="25" t="s">
+        <v>31</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="16"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1624,7 +1647,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
-      <c r="J10" s="16"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1644,31 +1667,31 @@
     </row>
     <row r="11">
       <c r="A11" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>13</v>
+      <c r="E11" s="13" t="s">
+        <v>14</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>15</v>
+      <c r="G11" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1687,22 +1710,24 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="16"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1730,7 +1755,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="16"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -1750,25 +1775,25 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="16"/>
+      <c r="H14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -1788,23 +1813,23 @@
     </row>
     <row r="15">
       <c r="A15" s="27"/>
-      <c r="B15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="13" t="s">
-        <v>29</v>
+      <c r="D15" s="18"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="17" t="s">
+        <v>47</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="16"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="20"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1824,21 +1849,21 @@
     </row>
     <row r="16">
       <c r="A16" s="29"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="18" t="s">
+      <c r="D16" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1866,7 +1891,7 @@
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
-      <c r="J17" s="16"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -1886,27 +1911,27 @@
     </row>
     <row r="18">
       <c r="A18" s="26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="13" t="s">
-        <v>51</v>
+      <c r="C18" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>13</v>
+      <c r="D18" s="12" t="s">
+        <v>52</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>26</v>
+      <c r="E18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>15</v>
-      </c>
+      <c r="H18" s="15"/>
       <c r="I18" s="31"/>
-      <c r="J18" s="16"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1927,22 +1952,22 @@
     <row r="19">
       <c r="A19" s="27"/>
       <c r="B19" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="25" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="16"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="15"/>
       <c r="K19" s="4"/>
       <c r="L19" s="33"/>
       <c r="M19" s="4"/>
@@ -1963,18 +1988,18 @@
     <row r="20">
       <c r="A20" s="34"/>
       <c r="B20" s="35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="36"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="16"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -2002,7 +2027,7 @@
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -2022,21 +2047,21 @@
     </row>
     <row r="22">
       <c r="A22" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="13" t="s">
-        <v>51</v>
+      <c r="B22" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="16"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -2055,18 +2080,18 @@
       <c r="Z22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="18" t="s">
-        <v>61</v>
+      <c r="C23" s="17" t="s">
+        <v>62</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="16"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="15"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -2085,18 +2110,16 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="17"/>
-      <c r="B24" s="13" t="s">
-        <v>62</v>
-      </c>
+      <c r="A24" s="16"/>
+      <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -2124,7 +2147,7 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
-      <c r="J25" s="16"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -2151,8 +2174,8 @@
         <v>64</v>
       </c>
       <c r="D26" s="36"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="42" t="s">
         <v>65</v>
       </c>
@@ -2160,7 +2183,7 @@
         <v>66</v>
       </c>
       <c r="I26" s="44"/>
-      <c r="J26" s="16"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -2183,20 +2206,24 @@
       <c r="B27" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="47" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="F27" s="48" t="s">
         <v>70</v>
       </c>
+      <c r="G27" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="I27" s="44"/>
-      <c r="J27" s="16"/>
+      <c r="J27" s="15"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -2215,24 +2242,28 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="48"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>74</v>
       </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="I28" s="44"/>
-      <c r="J28" s="16"/>
+      <c r="J28" s="15"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -2251,25 +2282,29 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="50"/>
-      <c r="B29" s="47" t="s">
-        <v>75</v>
+      <c r="A29" s="52"/>
+      <c r="B29" s="49" t="s">
+        <v>79</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>76</v>
+      <c r="C29" s="17" t="s">
+        <v>80</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="49" t="s">
-        <v>77</v>
+      <c r="D29" s="18"/>
+      <c r="E29" s="47" t="s">
+        <v>81</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>78</v>
+      <c r="F29" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="I29" s="44"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2287,24 +2322,24 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="50"/>
-      <c r="B30" s="47" t="s">
-        <v>79</v>
+      <c r="A30" s="52"/>
+      <c r="B30" s="49" t="s">
+        <v>85</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>80</v>
+      <c r="C30" s="17" t="s">
+        <v>86</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="51" t="s">
-        <v>81</v>
+      <c r="D30" s="18"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="53" t="s">
+        <v>87</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I30" s="44"/>
-      <c r="J30" s="16"/>
+      <c r="J30" s="15"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -2323,24 +2358,24 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="50"/>
-      <c r="B31" s="52" t="s">
-        <v>83</v>
+      <c r="A31" s="52"/>
+      <c r="B31" s="54" t="s">
+        <v>89</v>
       </c>
-      <c r="C31" s="53" t="s">
-        <v>84</v>
+      <c r="C31" s="55" t="s">
+        <v>90</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="51" t="s">
-        <v>85</v>
+      <c r="D31" s="18"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="53" t="s">
+        <v>91</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>86</v>
+      <c r="H31" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="I31" s="44"/>
-      <c r="J31" s="16"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -2359,24 +2394,24 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="50"/>
-      <c r="B32" s="47" t="s">
-        <v>87</v>
+      <c r="A32" s="52"/>
+      <c r="B32" s="49" t="s">
+        <v>93</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>88</v>
+      <c r="C32" s="17" t="s">
+        <v>94</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="49" t="s">
-        <v>89</v>
+      <c r="D32" s="18"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="51" t="s">
+        <v>95</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>90</v>
+      <c r="H32" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="I32" s="44"/>
-      <c r="J32" s="16"/>
+      <c r="J32" s="15"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -2395,24 +2430,24 @@
       <c r="Z32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="50"/>
-      <c r="B33" s="47" t="s">
-        <v>91</v>
+      <c r="A33" s="52"/>
+      <c r="B33" s="49" t="s">
+        <v>97</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>92</v>
+      <c r="C33" s="17" t="s">
+        <v>98</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="51" t="s">
-        <v>93</v>
+      <c r="D33" s="18"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="53" t="s">
+        <v>99</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>94</v>
+      <c r="H33" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="I33" s="44"/>
-      <c r="J33" s="16"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2431,24 +2466,24 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="50"/>
-      <c r="B34" s="54" t="s">
-        <v>95</v>
+      <c r="A34" s="52"/>
+      <c r="B34" s="56" t="s">
+        <v>101</v>
       </c>
-      <c r="C34" s="53" t="s">
-        <v>96</v>
+      <c r="C34" s="55" t="s">
+        <v>102</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="51" t="s">
-        <v>97</v>
+      <c r="D34" s="18"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="53" t="s">
+        <v>103</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>98</v>
+      <c r="H34" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="I34" s="44"/>
-      <c r="J34" s="16"/>
+      <c r="J34" s="15"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2467,24 +2502,24 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="50"/>
-      <c r="B35" s="54" t="s">
-        <v>99</v>
+      <c r="A35" s="52"/>
+      <c r="B35" s="56" t="s">
+        <v>105</v>
       </c>
-      <c r="C35" s="53" t="s">
-        <v>100</v>
+      <c r="C35" s="55" t="s">
+        <v>106</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="55" t="s">
-        <v>101</v>
+      <c r="D35" s="18"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="57" t="s">
+        <v>107</v>
       </c>
-      <c r="H35" s="56" t="s">
-        <v>102</v>
+      <c r="H35" s="58" t="s">
+        <v>108</v>
       </c>
       <c r="I35" s="44"/>
-      <c r="J35" s="16"/>
+      <c r="J35" s="15"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2503,20 +2538,20 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36">
-      <c r="A36" s="50"/>
-      <c r="B36" s="47" t="s">
-        <v>103</v>
+      <c r="A36" s="52"/>
+      <c r="B36" s="49" t="s">
+        <v>109</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>104</v>
+      <c r="C36" s="17" t="s">
+        <v>110</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="16"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="15"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2535,20 +2570,20 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="50"/>
-      <c r="B37" s="47" t="s">
-        <v>105</v>
+      <c r="A37" s="52"/>
+      <c r="B37" s="49" t="s">
+        <v>111</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>106</v>
+      <c r="C37" s="17" t="s">
+        <v>112</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="16"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2567,20 +2602,20 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="50"/>
-      <c r="B38" s="47" t="s">
-        <v>107</v>
+      <c r="A38" s="52"/>
+      <c r="B38" s="49" t="s">
+        <v>113</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>108</v>
+      <c r="C38" s="17" t="s">
+        <v>114</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="16"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="15"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2599,22 +2634,22 @@
       <c r="Z38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="50"/>
-      <c r="B39" s="52" t="s">
-        <v>109</v>
+      <c r="A39" s="52"/>
+      <c r="B39" s="54" t="s">
+        <v>115</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>110</v>
+      <c r="C39" s="17" t="s">
+        <v>116</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="59" t="s">
+      <c r="D39" s="18"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="57"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="16"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2633,20 +2668,20 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40">
-      <c r="A40" s="50"/>
-      <c r="B40" s="47" t="s">
-        <v>111</v>
+      <c r="A40" s="52"/>
+      <c r="B40" s="49" t="s">
+        <v>117</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>112</v>
+      <c r="C40" s="17" t="s">
+        <v>118</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="16"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2665,20 +2700,20 @@
       <c r="Z40" s="4"/>
     </row>
     <row r="41">
-      <c r="A41" s="50"/>
-      <c r="B41" s="47" t="s">
-        <v>113</v>
+      <c r="A41" s="52"/>
+      <c r="B41" s="49" t="s">
+        <v>119</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>114</v>
+      <c r="C41" s="17" t="s">
+        <v>120</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="16"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="15"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2697,9 +2732,9 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42">
-      <c r="A42" s="50"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2725,9 +2760,9 @@
       <c r="Z42" s="4"/>
     </row>
     <row r="43">
-      <c r="A43" s="50"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2753,9 +2788,9 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="50"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2781,9 +2816,9 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="50"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -2809,15 +2844,15 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="50"/>
-      <c r="B46" s="60" t="s">
-        <v>115</v>
+      <c r="A46" s="52"/>
+      <c r="B46" s="61" t="s">
+        <v>121</v>
       </c>
-      <c r="C46" s="50"/>
+      <c r="C46" s="52"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
-      <c r="F46" s="60" t="s">
-        <v>116</v>
+      <c r="F46" s="61" t="s">
+        <v>122</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -2841,28 +2876,28 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="16"/>
-      <c r="B47" s="61" t="s">
-        <v>117</v>
+      <c r="A47" s="15"/>
+      <c r="B47" s="62" t="s">
+        <v>123</v>
       </c>
-      <c r="C47" s="62" t="s">
-        <v>118</v>
+      <c r="C47" s="63" t="s">
+        <v>124</v>
       </c>
-      <c r="D47" s="63" t="s">
-        <v>119</v>
+      <c r="D47" s="64" t="s">
+        <v>125</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="64" t="s">
-        <v>120</v>
+      <c r="F47" s="65" t="s">
+        <v>126</v>
       </c>
-      <c r="G47" s="65" t="s">
-        <v>121</v>
+      <c r="G47" s="66" t="s">
+        <v>127</v>
       </c>
-      <c r="H47" s="66" t="s">
-        <v>122</v>
+      <c r="H47" s="67" t="s">
+        <v>128</v>
       </c>
-      <c r="I47" s="67" t="s">
-        <v>123</v>
+      <c r="I47" s="68" t="s">
+        <v>129</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -2883,26 +2918,26 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="16"/>
-      <c r="B48" s="68" t="s">
+      <c r="A48" s="15"/>
+      <c r="B48" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="C48" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="63" t="s">
-        <v>119</v>
+      <c r="D48" s="64" t="s">
+        <v>125</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="69" t="s">
-        <v>125</v>
+      <c r="F48" s="19"/>
+      <c r="G48" s="70" t="s">
+        <v>131</v>
       </c>
-      <c r="H48" s="66" t="s">
-        <v>122</v>
+      <c r="H48" s="67" t="s">
+        <v>128</v>
       </c>
-      <c r="I48" s="67" t="s">
-        <v>123</v>
+      <c r="I48" s="68" t="s">
+        <v>129</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -2923,28 +2958,28 @@
       <c r="Z48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="16"/>
-      <c r="B49" s="61" t="s">
-        <v>126</v>
+      <c r="A49" s="15"/>
+      <c r="B49" s="62" t="s">
+        <v>132</v>
       </c>
-      <c r="C49" s="70" t="s">
-        <v>118</v>
+      <c r="C49" s="71" t="s">
+        <v>124</v>
       </c>
-      <c r="D49" s="71" t="s">
-        <v>127</v>
+      <c r="D49" s="72" t="s">
+        <v>133</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="F49" s="72" t="s">
-        <v>128</v>
+      <c r="F49" s="73" t="s">
+        <v>134</v>
       </c>
-      <c r="G49" s="73" t="s">
-        <v>129</v>
+      <c r="G49" s="74" t="s">
+        <v>135</v>
       </c>
-      <c r="H49" s="74" t="s">
-        <v>118</v>
+      <c r="H49" s="75" t="s">
+        <v>124</v>
       </c>
-      <c r="I49" s="75" t="s">
-        <v>130</v>
+      <c r="I49" s="76" t="s">
+        <v>136</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -2965,20 +3000,20 @@
       <c r="Z49" s="4"/>
     </row>
     <row r="50">
-      <c r="A50" s="76"/>
-      <c r="B50" s="77"/>
-      <c r="C50" s="78"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="79"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="28"/>
-      <c r="G50" s="73" t="s">
-        <v>131</v>
+      <c r="G50" s="74" t="s">
+        <v>137</v>
       </c>
-      <c r="H50" s="74" t="s">
-        <v>118</v>
+      <c r="H50" s="75" t="s">
+        <v>124</v>
       </c>
-      <c r="I50" s="75" t="s">
-        <v>130</v>
+      <c r="I50" s="76" t="s">
+        <v>136</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -2999,20 +3034,20 @@
       <c r="Z50" s="4"/>
     </row>
     <row r="51">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="78"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="79"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="73" t="s">
-        <v>132</v>
+      <c r="F51" s="19"/>
+      <c r="G51" s="74" t="s">
+        <v>138</v>
       </c>
-      <c r="H51" s="74" t="s">
-        <v>118</v>
+      <c r="H51" s="75" t="s">
+        <v>124</v>
       </c>
-      <c r="I51" s="75" t="s">
-        <v>130</v>
+      <c r="I51" s="76" t="s">
+        <v>136</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -3033,9 +3068,9 @@
       <c r="Z51" s="4"/>
     </row>
     <row r="52">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="78"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="79"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -3061,9 +3096,9 @@
       <c r="Z52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="78"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="79"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -3071,7 +3106,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
-      <c r="K53" s="16"/>
+      <c r="K53" s="15"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
@@ -3089,7 +3124,7 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="16"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -3099,7 +3134,7 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
-      <c r="K54" s="16"/>
+      <c r="K54" s="15"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
@@ -3117,9 +3152,9 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55">
-      <c r="A55" s="16"/>
-      <c r="B55" s="79" t="s">
-        <v>133</v>
+      <c r="A55" s="15"/>
+      <c r="B55" s="80" t="s">
+        <v>139</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -3129,7 +3164,7 @@
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
-      <c r="K55" s="16"/>
+      <c r="K55" s="15"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
@@ -3147,16 +3182,16 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56">
-      <c r="A56" s="16"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="80" t="s">
-        <v>134</v>
+      <c r="C56" s="81" t="s">
+        <v>140</v>
       </c>
-      <c r="D56" s="81" t="s">
-        <v>118</v>
+      <c r="D56" s="82" t="s">
+        <v>124</v>
       </c>
-      <c r="E56" s="67" t="s">
-        <v>135</v>
+      <c r="E56" s="68" t="s">
+        <v>141</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -3181,16 +3216,16 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="16"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="80" t="s">
-        <v>136</v>
+      <c r="C57" s="81" t="s">
+        <v>142</v>
       </c>
-      <c r="D57" s="81" t="s">
-        <v>118</v>
+      <c r="D57" s="82" t="s">
+        <v>124</v>
       </c>
-      <c r="E57" s="67" t="s">
-        <v>137</v>
+      <c r="E57" s="68" t="s">
+        <v>143</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -3215,9 +3250,9 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="78"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="79"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -3243,9 +3278,9 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="78"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="79"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3271,9 +3306,9 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="78"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="79"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -3299,9 +3334,9 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="78"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="79"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3327,9 +3362,9 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="78"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="79"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3355,15 +3390,15 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="78"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="79"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
-      <c r="I63" s="82"/>
+      <c r="I63" s="83"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -3553,8 +3588,8 @@
     <row r="70">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -3581,8 +3616,8 @@
     <row r="71">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -3609,8 +3644,8 @@
     <row r="72">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
+      <c r="C72" s="52"/>
+      <c r="D72" s="52"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -3637,8 +3672,8 @@
     <row r="73">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="52"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -3665,8 +3700,8 @@
     <row r="74">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="52"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -3693,8 +3728,8 @@
     <row r="75">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="52"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -3721,8 +3756,8 @@
     <row r="76">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="52"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -3749,8 +3784,8 @@
     <row r="77">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
+      <c r="C77" s="52"/>
+      <c r="D77" s="52"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -3777,8 +3812,8 @@
     <row r="78">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
+      <c r="C78" s="52"/>
+      <c r="D78" s="52"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -3805,8 +3840,8 @@
     <row r="79">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
+      <c r="C79" s="52"/>
+      <c r="D79" s="52"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -3833,8 +3868,8 @@
     <row r="80">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="50"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="52"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -3861,8 +3896,8 @@
     <row r="81">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
+      <c r="C81" s="52"/>
+      <c r="D81" s="52"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -3889,8 +3924,8 @@
     <row r="82">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="52"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -3917,8 +3952,8 @@
     <row r="83">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
+      <c r="C83" s="52"/>
+      <c r="D83" s="52"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -3945,8 +3980,8 @@
     <row r="84">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
+      <c r="C84" s="52"/>
+      <c r="D84" s="52"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>

</xml_diff>

<commit_message>
chore: 11 aug updation 62 sem1,3 and bca
</commit_message>
<xml_diff>
--- a/raw/time_tables/BCA(bca-62)/3/1.xlsx
+++ b/raw/time_tables/BCA(bca-62)/3/1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="144">
   <si>
     <t>Bachelors of Computer Applications</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>LBCA1, BCA2(23B61CA211)-325/KSA</t>
+    <t>LBCA1, BCA2(23B61CA211)-CR-501/KSA</t>
   </si>
   <si>
     <t>LBCA3, BCA4(23B61CA213)-CR501/DCH</t>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>LBCA3, BCA4(23B31MA211)-CR301/NF3</t>
+  </si>
+  <si>
+    <t>PBCA3(23B65CA214)-CC423/KSA</t>
   </si>
   <si>
     <t>PBCA4(23B65CA215)-CC423/IMR,REK</t>
@@ -90,6 +93,9 @@
     <t>TBCA4(23B61CA212)-TR424/MEE</t>
   </si>
   <si>
+    <t>LBCA3, BCA4(23B61CA211)-CR325 KSA</t>
+  </si>
+  <si>
     <t>LBCA3, BCA4(23B61CA212)-CR301/SHO</t>
   </si>
   <si>
@@ -100,9 +106,6 @@
   </si>
   <si>
     <t>PBCA2(23B65CA216)-CL24/AKT</t>
-  </si>
-  <si>
-    <t>PBCA3(23B65CA214)-CC423/KSA</t>
   </si>
   <si>
     <t>LBCA1, BCA2(23B61CA213)-CR325/DCH</t>
@@ -117,6 +120,9 @@
     <t>LBCA1, BCA2(23B61CA212)-CR301/MEE</t>
   </si>
   <si>
+    <t>LBCA1, BCA2(23B61CA211)-325/KSA</t>
+  </si>
+  <si>
     <t>LBCA1, BCA2(23B31HS211)-CR301/SHU</t>
   </si>
   <si>
@@ -126,16 +132,10 @@
     <t>LBCA3,BCA4(23B61CA212)-CR501/SHO</t>
   </si>
   <si>
-    <t>LBCA3, BCA4(23B61CA211)-CR325 KSA</t>
-  </si>
-  <si>
     <t>PBCA3(23B65CA215)-CC423/MEE</t>
   </si>
   <si>
     <t>PBCA2(23B31HS211)-Computer Centre Room no 423 4th Floor ABB-III/SDA</t>
-  </si>
-  <si>
-    <t>LBCA1, BCA2(23B61CA211)-CR301/ KSA</t>
   </si>
   <si>
     <t>THUR</t>
@@ -191,7 +191,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-PBCA1(23B65CA214)-CC421/SHG</t>
+PBCA1(23B65CA214)-CC421/SHG , AKT</t>
   </si>
   <si>
     <t>PBCA2(23B65CA215)-CC417/MEE,AW</t>
@@ -239,7 +239,7 @@
     <t>KSA</t>
   </si>
   <si>
-    <t>Aakriti Bhardwaj</t>
+    <t>Kashav Ajmera</t>
   </si>
   <si>
     <t>BB</t>
@@ -632,17 +632,6 @@
       </top>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -663,6 +652,17 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
     </border>
     <border>
       <left style="thin">
@@ -746,24 +746,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -788,6 +770,24 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -923,32 +923,35 @@
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="14" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="7" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="17" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -957,6 +960,9 @@
     <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -966,29 +972,23 @@
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="24" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="24" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="22" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1009,14 +1009,14 @@
     <xf borderId="31" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="31" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="29" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="29" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1025,17 +1025,17 @@
     <xf borderId="31" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="29" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="29" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -1056,13 +1056,13 @@
     <xf borderId="7" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="24" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1086,10 +1086,10 @@
     <xf borderId="33" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1428,24 +1428,26 @@
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
+      <c r="H4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1464,24 +1466,24 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17" t="s">
-        <v>17</v>
+      <c r="A5" s="18"/>
+      <c r="B5" s="15" t="s">
+        <v>18</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="4"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="G5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="15"/>
+      <c r="H5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1500,20 +1502,20 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="12" t="s">
-        <v>21</v>
+      <c r="D6" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="17" t="s">
-        <v>22</v>
+      <c r="G6" s="15" t="s">
+        <v>23</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1532,16 +1534,16 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="15"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1560,30 +1562,32 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="17" t="s">
+      <c r="F8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="15"/>
+      <c r="G8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -1602,24 +1606,22 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="24"/>
-      <c r="B9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="12" t="s">
-        <v>30</v>
+      <c r="A9" s="25"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="25" t="s">
-        <v>31</v>
+      <c r="F9" s="26" t="s">
+        <v>32</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="12" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="20"/>
-      <c r="J9" s="15"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1638,16 +1640,16 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="15"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1666,32 +1668,32 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="C11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>35</v>
+      <c r="F11" s="13" t="s">
+        <v>37</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>36</v>
+      <c r="H11" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="I11" s="20"/>
-      <c r="J11" s="15"/>
+      <c r="J11" s="17"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1710,24 +1712,20 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="25" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="12" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="26" t="s">
         <v>40</v>
       </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="20"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="17"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1746,16 +1744,16 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="15"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="17"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -1774,26 +1772,26 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="13" t="s">
         <v>44</v>
       </c>
       <c r="I14" s="20"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -1812,24 +1810,24 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="17" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="12" t="s">
-        <v>30</v>
+      <c r="G15" s="16"/>
+      <c r="H15" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="I15" s="20"/>
-      <c r="J15" s="15"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -1848,22 +1846,22 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="29"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -1882,16 +1880,16 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="15"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="17"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -1910,28 +1908,28 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="15"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1950,26 +1948,26 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="28"/>
+      <c r="B19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="13" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="25" t="s">
+      <c r="G19" s="21"/>
+      <c r="H19" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="15"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="33"/>
+      <c r="L19" s="31"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1986,20 +1984,20 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="18"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="20"/>
-      <c r="J20" s="15"/>
+      <c r="J20" s="17"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -2018,16 +2016,16 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="15"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -2046,22 +2044,22 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="15"/>
+      <c r="J22" s="17"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -2080,18 +2078,18 @@
       <c r="Z22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="16"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="14"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="15"/>
+      <c r="J23" s="17"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -2110,16 +2108,16 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="14"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="20"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="17"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
@@ -2138,16 +2136,16 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="15"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="17"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -2166,14 +2164,14 @@
       <c r="Z25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="39"/>
-      <c r="B26" s="40" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="36"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="42" t="s">
@@ -2183,7 +2181,7 @@
         <v>66</v>
       </c>
       <c r="I26" s="44"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="17"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
@@ -2206,10 +2204,10 @@
       <c r="B27" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="18"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="47" t="s">
         <v>69</v>
       </c>
@@ -2219,11 +2217,11 @@
       <c r="G27" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="15" t="s">
         <v>72</v>
       </c>
       <c r="I27" s="44"/>
-      <c r="J27" s="15"/>
+      <c r="J27" s="17"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
@@ -2246,10 +2244,10 @@
       <c r="B28" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="18"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="47" t="s">
         <v>75</v>
       </c>
@@ -2259,11 +2257,11 @@
       <c r="G28" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="15" t="s">
         <v>78</v>
       </c>
       <c r="I28" s="44"/>
-      <c r="J28" s="15"/>
+      <c r="J28" s="17"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -2286,10 +2284,10 @@
       <c r="B29" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="18"/>
+      <c r="D29" s="16"/>
       <c r="E29" s="47" t="s">
         <v>81</v>
       </c>
@@ -2299,12 +2297,12 @@
       <c r="G29" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="15" t="s">
         <v>84</v>
       </c>
       <c r="I29" s="44"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2326,20 +2324,20 @@
       <c r="B30" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="18"/>
+      <c r="D30" s="16"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="37" t="s">
+      <c r="H30" s="36" t="s">
         <v>88</v>
       </c>
       <c r="I30" s="44"/>
-      <c r="J30" s="15"/>
+      <c r="J30" s="17"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
@@ -2365,17 +2363,17 @@
       <c r="C31" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="18"/>
+      <c r="D31" s="16"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="14"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="15" t="s">
         <v>92</v>
       </c>
       <c r="I31" s="44"/>
-      <c r="J31" s="15"/>
+      <c r="J31" s="17"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
@@ -2398,20 +2396,20 @@
       <c r="B32" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="16"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="14"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="15" t="s">
         <v>96</v>
       </c>
       <c r="I32" s="44"/>
-      <c r="J32" s="15"/>
+      <c r="J32" s="17"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
@@ -2434,20 +2432,20 @@
       <c r="B33" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="18"/>
+      <c r="D33" s="16"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="14"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="15" t="s">
         <v>100</v>
       </c>
       <c r="I33" s="44"/>
-      <c r="J33" s="15"/>
+      <c r="J33" s="17"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
@@ -2473,17 +2471,17 @@
       <c r="C34" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="15" t="s">
         <v>104</v>
       </c>
       <c r="I34" s="44"/>
-      <c r="J34" s="15"/>
+      <c r="J34" s="17"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2509,9 +2507,9 @@
       <c r="C35" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="18"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="14"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="57" t="s">
         <v>107</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>108</v>
       </c>
       <c r="I35" s="44"/>
-      <c r="J35" s="15"/>
+      <c r="J35" s="17"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2542,16 +2540,16 @@
       <c r="B36" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="18"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="59"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="15"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="17"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2574,16 +2572,16 @@
       <c r="B37" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C37" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="16"/>
       <c r="E37" s="20"/>
       <c r="F37" s="20"/>
       <c r="G37" s="60"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
-      <c r="J37" s="15"/>
+      <c r="J37" s="17"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2606,16 +2604,16 @@
       <c r="B38" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="59"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="15"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="17"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2638,18 +2636,18 @@
       <c r="B39" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="14"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="21"/>
       <c r="F39" s="48" t="s">
         <v>11</v>
       </c>
       <c r="G39" s="59"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="15"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="17"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2672,16 +2670,16 @@
       <c r="B40" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="59"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="15"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="17"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2704,16 +2702,16 @@
       <c r="B41" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="59"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="15"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="17"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2876,7 +2874,7 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="15"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="62" t="s">
         <v>123</v>
       </c>
@@ -2918,7 +2916,7 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="15"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="69" t="s">
         <v>130</v>
       </c>
@@ -2958,7 +2956,7 @@
       <c r="Z48" s="4"/>
     </row>
     <row r="49">
-      <c r="A49" s="15"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="62" t="s">
         <v>132</v>
       </c>
@@ -3005,7 +3003,7 @@
       <c r="C50" s="79"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
-      <c r="F50" s="28"/>
+      <c r="F50" s="29"/>
       <c r="G50" s="74" t="s">
         <v>137</v>
       </c>
@@ -3034,8 +3032,8 @@
       <c r="Z50" s="4"/>
     </row>
     <row r="51">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="79"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -3068,8 +3066,8 @@
       <c r="Z51" s="4"/>
     </row>
     <row r="52">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="79"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -3096,8 +3094,8 @@
       <c r="Z52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="79"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -3106,7 +3104,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
-      <c r="K53" s="15"/>
+      <c r="K53" s="17"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
@@ -3124,7 +3122,7 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="15"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -3134,7 +3132,7 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
-      <c r="K54" s="15"/>
+      <c r="K54" s="17"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
@@ -3152,7 +3150,7 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55">
-      <c r="A55" s="15"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="80" t="s">
         <v>139</v>
       </c>
@@ -3164,7 +3162,7 @@
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
-      <c r="K55" s="15"/>
+      <c r="K55" s="17"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
@@ -3182,7 +3180,7 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56">
-      <c r="A56" s="15"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="4"/>
       <c r="C56" s="81" t="s">
         <v>140</v>
@@ -3216,7 +3214,7 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="15"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="4"/>
       <c r="C57" s="81" t="s">
         <v>142</v>
@@ -3250,8 +3248,8 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
       <c r="C58" s="79"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -3278,8 +3276,8 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
       <c r="C59" s="79"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -3306,8 +3304,8 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="79"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -3334,8 +3332,8 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61">
-      <c r="A61" s="15"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="79"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3362,8 +3360,8 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="79"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -3390,8 +3388,8 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
       <c r="C63" s="79"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -29655,63 +29653,63 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="H32:I32"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="F47:F48"/>
     <mergeCell ref="F49:F51"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="H34:I34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E14:E16"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>